<commit_message>
add a new patient record to the excel
</commit_message>
<xml_diff>
--- a/src/main/resources/Patients.xlsx
+++ b/src/main/resources/Patients.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Imię</t>
   </si>
@@ -58,6 +58,12 @@
   <si>
     <t>840712948354</t>
   </si>
+  <si>
+    <t>Kowalski</t>
+  </si>
+  <si>
+    <t>0430403</t>
+  </si>
 </sst>
 </file>
 
@@ -101,7 +107,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -162,6 +168,17 @@
         <v>14</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
additional functionalities (bank account status, registration)
</commit_message>
<xml_diff>
--- a/src/main/resources/Patients.xlsx
+++ b/src/main/resources/Patients.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Imię</t>
   </si>
@@ -20,7 +20,7 @@
     <t>Nazwisko</t>
   </si>
   <si>
-    <t>PESEL</t>
+    <t>Pesel</t>
   </si>
   <si>
     <t>Piotr</t>
@@ -59,10 +59,19 @@
     <t>840712948354</t>
   </si>
   <si>
-    <t>Kowalski</t>
-  </si>
-  <si>
-    <t>0430403</t>
+    <t>Nowak</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Justyna</t>
+  </si>
+  <si>
+    <t>Justyńska</t>
+  </si>
+  <si>
+    <t>4949494</t>
   </si>
 </sst>
 </file>
@@ -107,7 +116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -170,13 +179,24 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
creating Excel with additional data
</commit_message>
<xml_diff>
--- a/src/main/resources/Patients.xlsx
+++ b/src/main/resources/Patients.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Imię</t>
   </si>
@@ -23,10 +23,10 @@
     <t>Pesel</t>
   </si>
   <si>
-    <t>Kwota wizyty</t>
-  </si>
-  <si>
-    <t>Zakażony</t>
+    <t>Portfel</t>
+  </si>
+  <si>
+    <t>Koronowirus</t>
   </si>
   <si>
     <t>Adam</t>
@@ -38,7 +38,7 @@
     <t>6565646</t>
   </si>
   <si>
-    <t>Brak Danych</t>
+    <t>brak</t>
   </si>
   <si>
     <t>Piotr</t>
@@ -59,6 +59,9 @@
     <t>534646564</t>
   </si>
   <si>
+    <t>negatywny</t>
+  </si>
+  <si>
     <t>Ada</t>
   </si>
   <si>
@@ -81,6 +84,9 @@
   </si>
   <si>
     <t>53400564</t>
+  </si>
+  <si>
+    <t>pozytywny</t>
   </si>
   <si>
     <t>Justyna</t>
@@ -134,7 +140,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -168,7 +174,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="n">
-        <v>400.0</v>
+        <v>50.0</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -185,7 +191,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="n">
-        <v>800.0</v>
+        <v>250.0</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -202,24 +208,24 @@
         <v>14</v>
       </c>
       <c r="D4" t="n">
-        <v>4000.0</v>
+        <v>2100.0</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" t="n">
-        <v>400.0</v>
+        <v>50.0</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -230,13 +236,13 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" t="n">
-        <v>1700.0</v>
+        <v>150.0</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -244,35 +250,52 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" t="n">
-        <v>4000.0</v>
+        <v>2100.0</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="n">
+        <v>2100.0</v>
+      </c>
+      <c r="E8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="D8" t="n">
-        <v>800.0</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="n">
+        <v>250.0</v>
+      </c>
+      <c r="E9" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>